<commit_message>
Finishing California and Colorado
</commit_message>
<xml_diff>
--- a/Avail_nClimDiv_LUT.xlsx
+++ b/Avail_nClimDiv_LUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA20AC5-DE64-834A-A7AD-B9E73CD8CFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA07A944-EAB1-1140-B0C8-AD519B25561F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16060" yWindow="1000" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13000" yWindow="2580" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avail_nClimDiv_LUT" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Status!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -570,7 +569,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -729,8 +728,17 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -922,6 +930,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1092,13 +1106,32 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4967,7 +5000,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -4975,7 +5008,7 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="29.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4988,386 +5021,386 @@
       <c r="C1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4">
-        <v>3200</v>
+        <v>100</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="C2" s="4">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4">
-        <v>3400</v>
+        <v>200</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C3" s="4">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4">
-        <v>3900</v>
+        <v>300</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C4" s="4">
         <v>9</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="9">
+        <v>400</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="9">
+        <v>500</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="9">
+        <v>5</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="11">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="11">
+        <v>6</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="11">
+        <v>1100</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="11">
+        <v>9</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="11">
+        <v>1200</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="11">
+        <v>6</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="11">
+        <v>1300</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="11">
+        <v>9</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="11">
+        <v>1400</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="11">
+        <v>9</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="11">
+        <v>1500</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4">
+        <v>2000</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="4">
+        <v>2100</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="4">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="4">
+        <v>2200</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4">
+        <v>2300</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="4">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4">
+        <v>2400</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="4">
+        <v>7</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4">
+        <v>2500</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="4">
+        <v>8</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4">
+        <v>2600</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" s="4">
+        <v>3</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4">
+        <v>2900</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="4">
+        <v>7</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3">
+        <v>3200</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="3">
+        <v>9</v>
+      </c>
+      <c r="D21" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4">
+    <row r="22" spans="1:4">
+      <c r="A22" s="3">
+        <v>3400</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="3">
+        <v>9</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3">
+        <v>3900</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="3">
+        <v>9</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3">
         <v>4000</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C24" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D24" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4">
+    <row r="25" spans="1:4">
+      <c r="A25" s="3">
         <v>4100</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C25" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D25" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4">
+    <row r="26" spans="1:4">
+      <c r="A26" s="3">
         <v>4200</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C26" s="3">
         <v>7</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D26" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4">
+    <row r="27" spans="1:4">
+      <c r="A27" s="3">
         <v>4700</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C27" s="3">
         <v>9</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D27" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4">
+    <row r="28" spans="1:4">
+      <c r="A28" s="3">
         <v>4800</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C28" s="3">
         <v>10</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D28" s="6">
         <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5">
-        <v>2000</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C10" s="5">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="5">
-        <v>2100</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="5">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="5">
-        <v>2200</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C12" s="5">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="5">
-        <v>2300</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="5">
-        <v>6</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="5">
-        <v>2400</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14" s="5">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="5">
-        <v>2500</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15" s="5">
-        <v>8</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="5">
-        <v>2600</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" s="5">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="5">
-        <v>2900</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="5">
-        <v>7</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="5">
-        <v>100</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" s="5">
-        <v>4</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="5">
-        <v>200</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C19" s="5">
-        <v>6</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="5">
-        <v>300</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" s="5">
-        <v>9</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="5">
-        <v>400</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="5">
-        <v>500</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C22" s="5">
-        <v>5</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="5">
-        <v>1000</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="5">
-        <v>6</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="5">
-        <v>1100</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C24" s="5">
-        <v>9</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="5">
-        <v>1200</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="5">
-        <v>6</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="5">
-        <v>1300</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="5">
-        <v>9</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="5">
-        <v>1400</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C27" s="5">
-        <v>9</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="5">
-        <v>1500</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" s="5">
-        <v>2</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5414,21 +5447,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
+    <row r="33" spans="1:4">
+      <c r="A33" s="3">
         <v>80000</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="3">
         <v>1</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{A3CC9153-DA2A-9649-A26A-D3C1B1D4FEE8}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
-      <sortCondition ref="D1:D33"/>
+      <sortCondition ref="A1:A33"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FIXING RETURN PERIOD CODE
</commit_message>
<xml_diff>
--- a/Avail_nClimDiv_LUT.xlsx
+++ b/Avail_nClimDiv_LUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CCFFE4-806B-6F42-AC5E-8193DADC610B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E0A35F-04D8-3E49-AE5F-97BCE3FD9C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="940" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="178">
   <si>
     <t>Full_Zone_Code</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>may need to redo 45</t>
+  </si>
+  <si>
+    <t>Cyclone</t>
   </si>
 </sst>
 </file>
@@ -741,7 +744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -951,6 +954,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1121,7 +1130,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1149,6 +1158,10 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5019,7 +5032,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -5307,7 +5320,7 @@
         <v>156</v>
       </c>
       <c r="C20" s="13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D20" s="14">
         <v>0</v>
@@ -5452,14 +5465,17 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="1">
+      <c r="A30" s="15">
         <v>40000</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="15">
         <v>6</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:5">

</xml_diff>

<commit_message>
bug fix in Loca CD Extreme event scriopts
</commit_message>
<xml_diff>
--- a/Avail_nClimDiv_LUT.xlsx
+++ b/Avail_nClimDiv_LUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E0A35F-04D8-3E49-AE5F-97BCE3FD9C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8140B291-C55D-A340-8447-34F29521E32A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="940" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,7 +744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -950,12 +950,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1156,12 +1150,12 @@
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5031,8 +5025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4F6AD8-E22E-E84B-9B31-F297ADD0EDD6}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -5296,16 +5290,16 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="13">
+      <c r="A19" s="15">
         <v>400</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="15">
         <v>1</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="16">
         <v>0</v>
       </c>
       <c r="E19" t="s">
@@ -5313,16 +5307,16 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="13">
+      <c r="A20" s="15">
         <v>500</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="15">
         <v>9</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="16">
         <v>0</v>
       </c>
       <c r="E20" t="s">
@@ -5465,16 +5459,16 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="15">
+      <c r="A30" s="13">
         <v>40000</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="13">
         <v>6</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="14" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>

<commit_message>
repairs to cd extreme analysis
</commit_message>
<xml_diff>
--- a/Avail_nClimDiv_LUT.xlsx
+++ b/Avail_nClimDiv_LUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02595A07-208C-294E-BC97-FE080EEA329F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61606481-DFF6-BF4D-8F20-3BE20E8BDAF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1000" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2360" yWindow="460" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avail_nClimDiv_LUT" sheetId="1" r:id="rId1"/>
@@ -5019,8 +5019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4F6AD8-E22E-E84B-9B31-F297ADD0EDD6}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>

</xml_diff>

<commit_message>
Adding a Separate Build Status Sheet
</commit_message>
<xml_diff>
--- a/Avail_nClimDiv_LUT.xlsx
+++ b/Avail_nClimDiv_LUT.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61606481-DFF6-BF4D-8F20-3BE20E8BDAF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA62BA9-E325-A841-A65A-88DA4D156AF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="460" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6760" yWindow="460" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avail_nClimDiv_LUT" sheetId="1" r:id="rId1"/>
-    <sheet name="Status" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Avail_nClimDiv_LUT!$A$1:$E$239</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Status!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="171">
   <si>
     <t>Full_Zone_Code</t>
   </si>
@@ -548,28 +546,13 @@
   </si>
   <si>
     <t>State Code</t>
-  </si>
-  <si>
-    <t>Freq</t>
-  </si>
-  <si>
-    <t>Machine</t>
-  </si>
-  <si>
-    <t>frost</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Cyclone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -704,41 +687,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -918,38 +868,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1064,15 +984,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1118,40 +1029,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1208,147 +1087,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6667500" cy="2882900"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE6FD091-0FAD-A744-B083-B72310D5173C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6070600" y="241300"/>
-          <a:ext cx="6667500" cy="2882900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Red:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Started Historical</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Orange:  Finished Historical </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Yellow; Finished RCP45 </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="92D050"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Green, Finished RCP85</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Blue, Archived in R</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" b="1" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" b="1" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" b="1" i="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Currently Running</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1650,7 +1388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D239"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -5013,472 +4751,4 @@
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4F6AD8-E22E-E84B-9B31-F297ADD0EDD6}">
-  <dimension ref="A1:D33"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="14.83203125" style="8" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3">
-        <v>3200</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="3">
-        <v>9</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3">
-        <v>3400</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="3">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3">
-        <v>3900</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3">
-        <v>4000</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="3">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3">
-        <v>4100</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="3">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3">
-        <v>4200</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" s="3">
-        <v>7</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3">
-        <v>4700</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" s="3">
-        <v>9</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3">
-        <v>4800</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C9" s="3">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3">
-        <v>80000</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="13">
-        <v>400</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="13">
-        <v>500</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="13">
-        <v>9</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="11">
-        <v>40000</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="11">
-        <v>6</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4">
-        <v>2000</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" s="4">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4">
-        <v>2100</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C15" s="4">
-        <v>9</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4">
-        <v>2200</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C16" s="4">
-        <v>5</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="4">
-        <v>2300</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C17" s="4">
-        <v>6</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="4">
-        <v>2400</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="4">
-        <v>7</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4">
-        <v>2500</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C19" s="4">
-        <v>8</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="4">
-        <v>2600</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="4">
-        <v>3</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="4">
-        <v>2900</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="4">
-        <v>7</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="9">
-        <v>100</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="9">
-        <v>4</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="9">
-        <v>200</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C23" s="9">
-        <v>6</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="9">
-        <v>300</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" s="9">
-        <v>9</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="15">
-        <v>1000</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="15">
-        <v>6</v>
-      </c>
-      <c r="D25" s="16"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="15">
-        <v>1100</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="15">
-        <v>9</v>
-      </c>
-      <c r="D26" s="16"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="15">
-        <v>1200</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C27" s="15">
-        <v>6</v>
-      </c>
-      <c r="D27" s="16"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="15">
-        <v>1300</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C28" s="15">
-        <v>9</v>
-      </c>
-      <c r="D28" s="16"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="15">
-        <v>1400</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C29" s="15">
-        <v>9</v>
-      </c>
-      <c r="D29" s="16"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="15">
-        <v>1500</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C30" s="15">
-        <v>2</v>
-      </c>
-      <c r="D30" s="16"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1">
-        <v>50000</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1">
-        <v>60000</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>70000</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="1">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{A3CC9153-DA2A-9649-A26A-D3C1B1D4FEE8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
-      <sortCondition ref="D1:D33"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>